<commit_message>
Corrections, Figure S4, Table S6
Correct ISUP labeling
</commit_message>
<xml_diff>
--- a/report/manuscript extras/pirads3_stats.xlsx
+++ b/report/manuscript extras/pirads3_stats.xlsx
@@ -527,7 +527,7 @@
         <v>0.6888888888888888</v>
       </c>
       <c r="C2">
-        <v>0.20647213690215</v>
+        <v>0.1597878787878788</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -559,7 +559,7 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="C4">
-        <v>0.625</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>